<commit_message>
sum of a column
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -159,7 +160,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,7 +195,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -434,7 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -491,4 +492,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>